<commit_message>
cells naming conventions, border and speed maps, excel lines fix
- fixed excel file line adding when excel file is already full but cell file doesnt exist.
- returned to the c and vt variable naming conventions as they are shorter and easier to use
- added border tuning-curve for x and y axes
- added speed tuning curve along with speed score (firing rate-speed correlation coef)
</commit_message>
<xml_diff>
--- a/inclusion_list_sessions.xlsx
+++ b/inclusion_list_sessions.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Scripts\nlxnlg_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{555A9B9C-FECD-4F4A-A15E-47EE1ED53F79}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69B10670-43A0-48B9-ABB4-BC7D7CC75ACC}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11490" tabRatio="306" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Experiments" sheetId="1" r:id="rId1"/>
-    <sheet name="Cells" sheetId="3" r:id="rId2"/>
+    <sheet name="Cells" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
@@ -14506,10 +14506,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1B0604F-4F37-4A96-8B06-7951C1BFFEA1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83412335-8C0C-4FBC-9738-0C3FEE48957E}">
   <dimension ref="A1:H941"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A916" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A916" workbookViewId="0">
       <selection activeCell="A941" sqref="A941:H941"/>
     </sheetView>
   </sheetViews>

</xml_diff>